<commit_message>
updated master sample sheet N=74
</commit_message>
<xml_diff>
--- a/Tapestri_batch2_samples_MASTER.xlsx
+++ b/Tapestri_batch2_samples_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/zhangh5_mskcc_org/Documents/Iacobuzio_lab/Tapestri_main_manuscript_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_AB229F4EB68DDA62DA4E72C19CE7FA089908D322" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67B0FD80-C177-CE46-B8E7-6DAA8172D45F}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="11_AB229F4EB68DDA62DA4E72C19CE7FA089908D322" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCD9B0E8-840B-7145-8508-68218E66B795}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="26460" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="567">
   <si>
     <t>Project Specific ID</t>
   </si>
@@ -1978,6 +1978,9 @@
   </si>
   <si>
     <t>PA4-2</t>
+  </si>
+  <si>
+    <t>M12-2</t>
   </si>
 </sst>
 </file>
@@ -7727,7 +7730,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8334,7 +8337,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>42</v>
+        <v>566</v>
       </c>
       <c r="C9" s="21">
         <v>0</v>

</xml_diff>